<commit_message>
update meeting minute and tasksheet
</commit_message>
<xml_diff>
--- a/Team/Task Sheet/TaskSheet .xlsx
+++ b/Team/Task Sheet/TaskSheet .xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6060" yWindow="1320" windowWidth="28160" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="6160" yWindow="1360" windowWidth="28160" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="46">
   <si>
     <t>Product Deliverables</t>
   </si>
@@ -123,12 +123,60 @@
   <si>
     <t xml:space="preserve">     Task sheet</t>
   </si>
+  <si>
+    <t>System Requirement Specification</t>
+  </si>
+  <si>
+    <t>List Of Use Case:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     External Interface Requirement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     System Overview Use case</t>
+  </si>
+  <si>
+    <t>Software System Attribute</t>
+  </si>
+  <si>
+    <t>Conceptual Diagram</t>
+  </si>
+  <si>
+    <t>Report 3 - Software Requirement Specification</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>Function Types</t>
+  </si>
+  <si>
+    <t>Function Point Size</t>
+  </si>
+  <si>
+    <t>Insert, Delete, Update, Simple Search, Login, Register, simple function or simple query on one table</t>
+  </si>
+  <si>
+    <t>Computed functions or joined query</t>
+  </si>
+  <si>
+    <t>Complex functions or multiple subquery</t>
+  </si>
+  <si>
+    <t>Constraint process and data integrity</t>
+  </si>
+  <si>
+    <t>Functions with implementing algorithms</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -210,6 +258,17 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Cambria"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Cambria"/>
     </font>
   </fonts>
@@ -305,7 +364,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -332,10 +391,13 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -345,8 +407,22 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -634,10 +710,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H31"/>
+  <dimension ref="A1:H89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -673,7 +749,7 @@
       </c>
     </row>
     <row r="2" spans="2:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -690,7 +766,7 @@
       </c>
     </row>
     <row r="3" spans="2:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="B3" s="10"/>
+      <c r="B3" s="12"/>
       <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
@@ -705,7 +781,7 @@
       </c>
     </row>
     <row r="4" spans="2:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="B4" s="10"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
@@ -720,7 +796,7 @@
       </c>
     </row>
     <row r="5" spans="2:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="B5" s="10"/>
+      <c r="B5" s="12"/>
       <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
@@ -731,7 +807,7 @@
       <c r="H5" s="6"/>
     </row>
     <row r="6" spans="2:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="B6" s="10"/>
+      <c r="B6" s="12"/>
       <c r="C6" s="3" t="s">
         <v>12</v>
       </c>
@@ -746,7 +822,7 @@
       </c>
     </row>
     <row r="7" spans="2:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="B7" s="10"/>
+      <c r="B7" s="12"/>
       <c r="C7" s="3" t="s">
         <v>13</v>
       </c>
@@ -761,7 +837,7 @@
       </c>
     </row>
     <row r="8" spans="2:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="B8" s="10"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="3" t="s">
         <v>14</v>
       </c>
@@ -776,7 +852,7 @@
       </c>
     </row>
     <row r="9" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="10"/>
+      <c r="B9" s="12"/>
       <c r="C9" s="3" t="s">
         <v>15</v>
       </c>
@@ -791,20 +867,20 @@
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
+      <c r="H10" s="17"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="13"/>
+      <c r="B11" s="14"/>
       <c r="C11" s="9" t="s">
         <v>21</v>
       </c>
@@ -814,21 +890,21 @@
         <v>8</v>
       </c>
       <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
+      <c r="H11" s="17"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B12" s="13"/>
-      <c r="C12" s="11" t="s">
+      <c r="B12" s="14"/>
+      <c r="C12" s="10" t="s">
         <v>18</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
+      <c r="H12" s="17"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B13" s="13"/>
+      <c r="B13" s="14"/>
       <c r="C13" s="9" t="s">
         <v>22</v>
       </c>
@@ -838,10 +914,10 @@
         <v>8</v>
       </c>
       <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
+      <c r="H13" s="17"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B14" s="13"/>
+      <c r="B14" s="14"/>
       <c r="C14" s="9" t="s">
         <v>23</v>
       </c>
@@ -851,22 +927,22 @@
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
+      <c r="H14" s="17"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B15" s="13"/>
+      <c r="B15" s="14"/>
       <c r="C15" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E15" s="9"/>
-      <c r="F15" s="15" t="s">
+      <c r="F15" s="11" t="s">
         <v>8</v>
       </c>
       <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
+      <c r="H15" s="17"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B16" s="13"/>
+      <c r="B16" s="14"/>
       <c r="C16" s="9" t="s">
         <v>25</v>
       </c>
@@ -876,10 +952,10 @@
       <c r="G16" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H16" s="9"/>
+      <c r="H16" s="17"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B17" s="13"/>
+      <c r="B17" s="14"/>
       <c r="C17" s="9" t="s">
         <v>26</v>
       </c>
@@ -889,34 +965,34 @@
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
+      <c r="H17" s="17"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B18" s="13"/>
+      <c r="B18" s="14"/>
       <c r="C18" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
+      <c r="H18" s="17"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B19" s="13"/>
-      <c r="C19" s="11" t="s">
+      <c r="B19" s="14"/>
+      <c r="C19" s="10" t="s">
         <v>20</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
+      <c r="H19" s="17"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B20" s="13"/>
+      <c r="B20" s="14"/>
       <c r="C20" s="9" t="s">
         <v>27</v>
       </c>
@@ -926,10 +1002,10 @@
       </c>
       <c r="F20" s="9"/>
       <c r="G20" s="5"/>
-      <c r="H20" s="9"/>
+      <c r="H20" s="17"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B21" s="13"/>
+      <c r="B21" s="14"/>
       <c r="C21" s="9" t="s">
         <v>28</v>
       </c>
@@ -939,10 +1015,10 @@
       <c r="G21" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H21" s="9"/>
+      <c r="H21" s="17"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B22" s="13"/>
+      <c r="B22" s="14"/>
       <c r="C22" s="9" t="s">
         <v>29</v>
       </c>
@@ -952,10 +1028,10 @@
       <c r="G22" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H22" s="9"/>
+      <c r="H22" s="17"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B23" s="14"/>
+      <c r="B23" s="15"/>
       <c r="C23" s="9" t="s">
         <v>15</v>
       </c>
@@ -965,84 +1041,604 @@
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
+      <c r="H23" s="17"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
+      <c r="B24" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>30</v>
+      </c>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
+      <c r="H24" s="17"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>8</v>
+      </c>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
+      <c r="H25" s="17"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="9" t="s">
+        <v>33</v>
+      </c>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
+      <c r="F26" s="8" t="s">
+        <v>8</v>
+      </c>
       <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
+      <c r="H26" s="17"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
+      <c r="H27" s="17"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="10"/>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
+      <c r="H28" s="17"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="10"/>
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
+      <c r="H29" s="17"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="10"/>
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
+      <c r="H30" s="17"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="10"/>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
+      <c r="H31" s="17"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B32" s="14"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="17"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B33" s="14"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="17"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B34" s="14"/>
+      <c r="C34" s="10"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="17"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B35" s="14"/>
+      <c r="C35" s="10"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="17"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B36" s="14"/>
+      <c r="C36" s="10"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="17"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B37" s="14"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="17"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B38" s="14"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="18"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B39" s="14"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="18"/>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B40" s="14"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="16"/>
+      <c r="H40" s="18"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B41" s="14"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="18"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B42" s="14"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="18"/>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B43" s="14"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="18"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B44" s="14"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="17"/>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B45" s="14"/>
+      <c r="C45" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
+      <c r="H45" s="17"/>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B46" s="14"/>
+      <c r="C46" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="17"/>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B47" s="14"/>
+      <c r="C47" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="17"/>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B48" s="14"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+      <c r="H48" s="17"/>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B49" s="14"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
+      <c r="H49" s="17"/>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B50" s="14"/>
+      <c r="C50" s="16"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="17"/>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B51" s="15"/>
+      <c r="C51" s="16"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="17"/>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B52" s="9"/>
+      <c r="C52" s="16"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="9"/>
+      <c r="G52" s="9"/>
+      <c r="H52" s="17"/>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B53" s="9"/>
+      <c r="C53" s="16"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="9"/>
+      <c r="H53" s="17"/>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B54" s="9"/>
+      <c r="C54" s="16"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="9"/>
+      <c r="H54" s="17"/>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B55" s="9"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="9"/>
+      <c r="G55" s="9"/>
+      <c r="H55" s="17"/>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B56" s="9"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="9"/>
+      <c r="G56" s="9"/>
+      <c r="H56" s="17"/>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B57" s="9"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
+      <c r="G57" s="9"/>
+      <c r="H57" s="17"/>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B58" s="9"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
+      <c r="G58" s="9"/>
+      <c r="H58" s="17"/>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B59" s="9"/>
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="9"/>
+      <c r="G59" s="9"/>
+      <c r="H59" s="17"/>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B60" s="9"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="9"/>
+      <c r="G60" s="9"/>
+      <c r="H60" s="17"/>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B61" s="9"/>
+      <c r="C61" s="9"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="9"/>
+      <c r="G61" s="9"/>
+      <c r="H61" s="17"/>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B62" s="9"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="9"/>
+      <c r="F62" s="9"/>
+      <c r="G62" s="9"/>
+      <c r="H62" s="17"/>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B63" s="9"/>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="9"/>
+      <c r="G63" s="9"/>
+      <c r="H63" s="17"/>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B64" s="9"/>
+      <c r="C64" s="9"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="9"/>
+      <c r="F64" s="9"/>
+      <c r="G64" s="9"/>
+      <c r="H64" s="17"/>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B65" s="9"/>
+      <c r="C65" s="9"/>
+      <c r="D65" s="9"/>
+      <c r="E65" s="9"/>
+      <c r="F65" s="9"/>
+      <c r="G65" s="9"/>
+      <c r="H65" s="17"/>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B66" s="9"/>
+      <c r="C66" s="9"/>
+      <c r="D66" s="9"/>
+      <c r="E66" s="9"/>
+      <c r="F66" s="9"/>
+      <c r="G66" s="9"/>
+      <c r="H66" s="17"/>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B67" s="9"/>
+      <c r="C67" s="9"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="9"/>
+      <c r="F67" s="9"/>
+      <c r="G67" s="9"/>
+      <c r="H67" s="17"/>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B68" s="9"/>
+      <c r="C68" s="9"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="9"/>
+      <c r="F68" s="9"/>
+      <c r="G68" s="9"/>
+      <c r="H68" s="9"/>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B69" s="9"/>
+      <c r="C69" s="9"/>
+      <c r="D69" s="9"/>
+      <c r="E69" s="9"/>
+      <c r="F69" s="9"/>
+      <c r="G69" s="9"/>
+      <c r="H69" s="9"/>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B70" s="9"/>
+      <c r="C70" s="9"/>
+      <c r="D70" s="9"/>
+      <c r="E70" s="9"/>
+      <c r="F70" s="9"/>
+      <c r="G70" s="9"/>
+      <c r="H70" s="9"/>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B71" s="9"/>
+      <c r="C71" s="9"/>
+      <c r="D71" s="9"/>
+      <c r="E71" s="9"/>
+      <c r="F71" s="9"/>
+      <c r="G71" s="9"/>
+      <c r="H71" s="9"/>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B72" s="9"/>
+      <c r="C72" s="9"/>
+      <c r="D72" s="9"/>
+      <c r="E72" s="9"/>
+      <c r="F72" s="9"/>
+      <c r="G72" s="9"/>
+      <c r="H72" s="9"/>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B73" s="9"/>
+      <c r="C73" s="9"/>
+      <c r="D73" s="9"/>
+      <c r="E73" s="9"/>
+      <c r="F73" s="9"/>
+      <c r="G73" s="9"/>
+      <c r="H73" s="9"/>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B74" s="9"/>
+      <c r="C74" s="9"/>
+      <c r="D74" s="9"/>
+      <c r="E74" s="9"/>
+      <c r="F74" s="9"/>
+      <c r="G74" s="9"/>
+      <c r="H74" s="9"/>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B75" s="9"/>
+      <c r="C75" s="9"/>
+      <c r="D75" s="9"/>
+      <c r="E75" s="9"/>
+      <c r="F75" s="9"/>
+      <c r="G75" s="9"/>
+      <c r="H75" s="9"/>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B76" s="9"/>
+      <c r="C76" s="9"/>
+      <c r="D76" s="9"/>
+      <c r="E76" s="9"/>
+      <c r="F76" s="9"/>
+      <c r="G76" s="9"/>
+      <c r="H76" s="9"/>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B77" s="9"/>
+      <c r="C77" s="9"/>
+      <c r="D77" s="9"/>
+      <c r="E77" s="9"/>
+      <c r="F77" s="9"/>
+      <c r="G77" s="9"/>
+      <c r="H77" s="9"/>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B78" s="9"/>
+      <c r="C78" s="9"/>
+      <c r="D78" s="9"/>
+      <c r="E78" s="9"/>
+      <c r="F78" s="9"/>
+      <c r="G78" s="9"/>
+      <c r="H78" s="9"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B83" s="20"/>
+      <c r="C83" s="21"/>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B84" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C84" s="23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A85" s="22">
+        <v>1</v>
+      </c>
+      <c r="B85" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C85" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" s="23">
+        <v>2</v>
+      </c>
+      <c r="B86" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="C86" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A87" s="23">
+        <v>3</v>
+      </c>
+      <c r="B87" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C87" s="23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" s="23">
+        <v>4</v>
+      </c>
+      <c r="B88" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C88" s="23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A89" s="23">
+        <v>5</v>
+      </c>
+      <c r="B89" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="C89" s="23">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B2:B9"/>
     <mergeCell ref="B10:B23"/>
+    <mergeCell ref="B24:B51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
update task sheet for report 3
</commit_message>
<xml_diff>
--- a/Team/Task Sheet/TaskSheet .xlsx
+++ b/Team/Task Sheet/TaskSheet .xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6160" yWindow="1360" windowWidth="28160" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="3380" yWindow="500" windowWidth="28160" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="85">
   <si>
     <t>Product Deliverables</t>
   </si>
@@ -171,12 +171,170 @@
   <si>
     <t>Functions with implementing algorithms</t>
   </si>
+  <si>
+    <t>User Requirement Specification</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>staff requirement</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">      bus driver requirement</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>customer requirement</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">     &lt;Guest&gt; Login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     &lt;Staff&gt; Logout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     &lt;Staff&gt; View Bus Route Information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     &lt;Staff&gt; View Bus Timetable Information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     &lt;Staff&gt; Edit Bus Route Information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     &lt;Staff&gt; Edit Bus Timtable Information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     &lt;Staff&gt; View configuration setting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     &lt;Staff&gt;  View system notifications</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      &lt;Staff&gt; Approve a notification </t>
+  </si>
+  <si>
+    <t xml:space="preserve">      &lt;Staff&gt; Reject a notification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      &lt;Staff&gt; Change Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      &lt;Staff&gt; Block one kind of notification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     &lt;Staff&gt; Config parser for getting data source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     &lt;Staff&gt; Config parser for prevent update one route</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      &lt;Customer&gt; view current location on mobile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      &lt;Customer&gt; view search history on mobile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       &lt;Customer&gt; synchronize data with server on mobile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       &lt;Customer&gt; view bus timetable on mobile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      &lt;Customer&gt; view bus route on mobile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       &lt;Customer&gt; search bus route on mobile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       &lt;Customer&gt; search motorbike route on mobile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       &lt;Customer&gt; view current location on wear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       &lt;Customer&gt; view list of all routes on wear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       &lt;Customer&gt; notification at station user need to leave on wear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       &lt;Customer&gt; notification when user need to turn on motorbike on wear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       &lt;Customer&gt; pair with mobile on wear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       &lt;Customer&gt; unpair with mobile on wear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       &lt;Customer&gt; pair with wear on mobile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       &lt;Customer&gt; unpair with wear on mobile</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">      &lt;Staff&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>View single notification</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">       &lt;bus driver&gt; view arrival data at each station</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       &lt;bus driver&gt; synchronize data to server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       &lt;bus driver&gt; get arrival time at each station</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       &lt;Customer&gt; search location and show on map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       &lt;Customer&gt; save user search history </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -271,6 +429,11 @@
       <color theme="1"/>
       <name val="Cambria"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -361,69 +524,69 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -710,16 +873,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H89"/>
+  <dimension ref="A1:H104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="E86" sqref="E86"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="33" customWidth="1"/>
-    <col min="3" max="3" width="37" customWidth="1"/>
+    <col min="3" max="3" width="57.33203125" customWidth="1"/>
     <col min="4" max="4" width="12.83203125" customWidth="1"/>
     <col min="5" max="5" width="13.83203125" customWidth="1"/>
     <col min="6" max="6" width="12.83203125" customWidth="1"/>
@@ -749,7 +912,7 @@
       </c>
     </row>
     <row r="2" spans="2:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="20" t="s">
         <v>16</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -766,7 +929,7 @@
       </c>
     </row>
     <row r="3" spans="2:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="B3" s="12"/>
+      <c r="B3" s="20"/>
       <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
@@ -781,7 +944,7 @@
       </c>
     </row>
     <row r="4" spans="2:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="B4" s="12"/>
+      <c r="B4" s="20"/>
       <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
@@ -796,7 +959,7 @@
       </c>
     </row>
     <row r="5" spans="2:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="B5" s="12"/>
+      <c r="B5" s="20"/>
       <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
@@ -807,7 +970,7 @@
       <c r="H5" s="6"/>
     </row>
     <row r="6" spans="2:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="B6" s="12"/>
+      <c r="B6" s="20"/>
       <c r="C6" s="3" t="s">
         <v>12</v>
       </c>
@@ -822,7 +985,7 @@
       </c>
     </row>
     <row r="7" spans="2:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="B7" s="12"/>
+      <c r="B7" s="20"/>
       <c r="C7" s="3" t="s">
         <v>13</v>
       </c>
@@ -837,7 +1000,7 @@
       </c>
     </row>
     <row r="8" spans="2:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="B8" s="12"/>
+      <c r="B8" s="20"/>
       <c r="C8" s="3" t="s">
         <v>14</v>
       </c>
@@ -852,7 +1015,7 @@
       </c>
     </row>
     <row r="9" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="12"/>
+      <c r="B9" s="20"/>
       <c r="C9" s="3" t="s">
         <v>15</v>
       </c>
@@ -867,7 +1030,7 @@
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="21" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="10" t="s">
@@ -877,10 +1040,10 @@
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
-      <c r="H10" s="17"/>
+      <c r="H10" s="13"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="14"/>
+      <c r="B11" s="22"/>
       <c r="C11" s="9" t="s">
         <v>21</v>
       </c>
@@ -890,10 +1053,10 @@
         <v>8</v>
       </c>
       <c r="G11" s="9"/>
-      <c r="H11" s="17"/>
+      <c r="H11" s="13"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B12" s="14"/>
+      <c r="B12" s="22"/>
       <c r="C12" s="10" t="s">
         <v>18</v>
       </c>
@@ -901,10 +1064,10 @@
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
-      <c r="H12" s="17"/>
+      <c r="H12" s="13"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B13" s="14"/>
+      <c r="B13" s="22"/>
       <c r="C13" s="9" t="s">
         <v>22</v>
       </c>
@@ -914,10 +1077,10 @@
         <v>8</v>
       </c>
       <c r="G13" s="9"/>
-      <c r="H13" s="17"/>
+      <c r="H13" s="13"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B14" s="14"/>
+      <c r="B14" s="22"/>
       <c r="C14" s="9" t="s">
         <v>23</v>
       </c>
@@ -927,10 +1090,10 @@
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
-      <c r="H14" s="17"/>
+      <c r="H14" s="13"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B15" s="14"/>
+      <c r="B15" s="22"/>
       <c r="C15" s="9" t="s">
         <v>24</v>
       </c>
@@ -939,10 +1102,10 @@
         <v>8</v>
       </c>
       <c r="G15" s="9"/>
-      <c r="H15" s="17"/>
+      <c r="H15" s="13"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B16" s="14"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="9" t="s">
         <v>25</v>
       </c>
@@ -952,10 +1115,10 @@
       <c r="G16" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H16" s="17"/>
+      <c r="H16" s="13"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B17" s="14"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="9" t="s">
         <v>26</v>
       </c>
@@ -965,10 +1128,10 @@
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
-      <c r="H17" s="17"/>
+      <c r="H17" s="13"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B18" s="14"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="9" t="s">
         <v>19</v>
       </c>
@@ -978,10 +1141,10 @@
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
-      <c r="H18" s="17"/>
+      <c r="H18" s="13"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B19" s="14"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="10" t="s">
         <v>20</v>
       </c>
@@ -989,10 +1152,10 @@
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
-      <c r="H19" s="17"/>
+      <c r="H19" s="13"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B20" s="14"/>
+      <c r="B20" s="22"/>
       <c r="C20" s="9" t="s">
         <v>27</v>
       </c>
@@ -1002,10 +1165,10 @@
       </c>
       <c r="F20" s="9"/>
       <c r="G20" s="5"/>
-      <c r="H20" s="17"/>
+      <c r="H20" s="13"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B21" s="14"/>
+      <c r="B21" s="22"/>
       <c r="C21" s="9" t="s">
         <v>28</v>
       </c>
@@ -1015,10 +1178,10 @@
       <c r="G21" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H21" s="17"/>
+      <c r="H21" s="13"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B22" s="14"/>
+      <c r="B22" s="22"/>
       <c r="C22" s="9" t="s">
         <v>29</v>
       </c>
@@ -1028,10 +1191,10 @@
       <c r="G22" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H22" s="17"/>
+      <c r="H22" s="13"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B23" s="15"/>
+      <c r="B23" s="23"/>
       <c r="C23" s="9" t="s">
         <v>15</v>
       </c>
@@ -1041,25 +1204,25 @@
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
-      <c r="H23" s="17"/>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B24" s="13" t="s">
+      <c r="H23" s="13"/>
+    </row>
+    <row r="24" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="21" t="s">
         <v>36</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
-      <c r="H24" s="17"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B25" s="14"/>
-      <c r="C25" s="9" t="s">
-        <v>32</v>
+      <c r="H24" s="13"/>
+    </row>
+    <row r="25" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="22"/>
+      <c r="C25" s="10" t="s">
+        <v>49</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>8</v>
@@ -1067,418 +1230,577 @@
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
-      <c r="H25" s="17"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B26" s="14"/>
-      <c r="C26" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="9"/>
+      <c r="H25" s="13"/>
+    </row>
+    <row r="26" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="22"/>
+      <c r="C26" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>8</v>
+      </c>
       <c r="E26" s="9"/>
-      <c r="F26" s="8" t="s">
-        <v>8</v>
-      </c>
+      <c r="F26" s="9"/>
       <c r="G26" s="9"/>
-      <c r="H26" s="17"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B27" s="14"/>
-      <c r="C27" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D27" s="9"/>
+      <c r="H26" s="13"/>
+    </row>
+    <row r="27" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="22"/>
+      <c r="C27" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>8</v>
+      </c>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
-      <c r="H27" s="17"/>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B28" s="14"/>
-      <c r="C28" s="10"/>
+      <c r="H27" s="13"/>
+    </row>
+    <row r="28" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="22"/>
+      <c r="C28" s="10" t="s">
+        <v>30</v>
+      </c>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
-      <c r="H28" s="17"/>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B29" s="14"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="9"/>
+      <c r="H28" s="13"/>
+    </row>
+    <row r="29" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="22"/>
+      <c r="C29" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>8</v>
+      </c>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
-      <c r="H29" s="17"/>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B30" s="14"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="9"/>
+      <c r="H29" s="13"/>
+    </row>
+    <row r="30" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="22"/>
+      <c r="C30" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>8</v>
+      </c>
       <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
+      <c r="F30" s="8" t="s">
+        <v>8</v>
+      </c>
       <c r="G30" s="9"/>
-      <c r="H30" s="17"/>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B31" s="14"/>
-      <c r="C31" s="10"/>
+      <c r="H30" s="13"/>
+    </row>
+    <row r="31" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="22"/>
+      <c r="C31" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="17"/>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B32" s="14"/>
-      <c r="C32" s="10"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="13"/>
+    </row>
+    <row r="32" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="22"/>
+      <c r="C32" s="12" t="s">
+        <v>50</v>
+      </c>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
       <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="17"/>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B33" s="14"/>
-      <c r="C33" s="10"/>
+      <c r="G32" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H32" s="13"/>
+    </row>
+    <row r="33" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="22"/>
+      <c r="C33" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="D33" s="9"/>
       <c r="E33" s="9"/>
       <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="17"/>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B34" s="14"/>
-      <c r="C34" s="10"/>
+      <c r="G33" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H33" s="13"/>
+    </row>
+    <row r="34" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="22"/>
+      <c r="C34" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D34" s="9"/>
       <c r="E34" s="9"/>
       <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="17"/>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B35" s="14"/>
-      <c r="C35" s="10"/>
+      <c r="G34" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H34" s="13"/>
+    </row>
+    <row r="35" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="22"/>
+      <c r="C35" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" s="9"/>
       <c r="E35" s="9"/>
       <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="17"/>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B36" s="14"/>
-      <c r="C36" s="10"/>
+      <c r="G35" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H35" s="13"/>
+    </row>
+    <row r="36" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="22"/>
+      <c r="C36" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D36" s="9"/>
       <c r="E36" s="9"/>
       <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="17"/>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B37" s="14"/>
-      <c r="C37" s="10"/>
+      <c r="G36" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H36" s="13"/>
+    </row>
+    <row r="37" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="22"/>
+      <c r="C37" s="12" t="s">
+        <v>54</v>
+      </c>
       <c r="D37" s="9"/>
       <c r="E37" s="9"/>
       <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="17"/>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B38" s="14"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="18"/>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B39" s="14"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="16"/>
-      <c r="G39" s="16"/>
-      <c r="H39" s="18"/>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B40" s="14"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="16"/>
-      <c r="E40" s="16"/>
-      <c r="F40" s="16"/>
-      <c r="G40" s="16"/>
-      <c r="H40" s="18"/>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B41" s="14"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="16"/>
-      <c r="E41" s="16"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="16"/>
-      <c r="H41" s="18"/>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B42" s="14"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="16"/>
-      <c r="E42" s="16"/>
-      <c r="F42" s="16"/>
-      <c r="G42" s="16"/>
-      <c r="H42" s="18"/>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B43" s="14"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="16"/>
-      <c r="E43" s="16"/>
-      <c r="F43" s="16"/>
-      <c r="G43" s="16"/>
-      <c r="H43" s="18"/>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B44" s="14"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9"/>
-      <c r="H44" s="17"/>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B45" s="14"/>
-      <c r="C45" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
-      <c r="H45" s="17"/>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B46" s="14"/>
-      <c r="C46" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-      <c r="H46" s="17"/>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B47" s="14"/>
-      <c r="C47" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E47" s="9"/>
+      <c r="G37" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H37" s="13"/>
+    </row>
+    <row r="38" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="22"/>
+      <c r="C38" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H38" s="13"/>
+    </row>
+    <row r="39" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="22"/>
+      <c r="C39" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H39" s="13"/>
+    </row>
+    <row r="40" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="22"/>
+      <c r="C40" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H40" s="13"/>
+    </row>
+    <row r="41" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="22"/>
+      <c r="C41" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H41" s="14"/>
+    </row>
+    <row r="42" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="22"/>
+      <c r="C42" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H42" s="14"/>
+    </row>
+    <row r="43" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="22"/>
+      <c r="C43" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H43" s="14"/>
+    </row>
+    <row r="44" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B44" s="22"/>
+      <c r="C44" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H44" s="14"/>
+    </row>
+    <row r="45" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="22"/>
+      <c r="C45" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H45" s="14"/>
+    </row>
+    <row r="46" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="22"/>
+      <c r="C46" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H46" s="14"/>
+    </row>
+    <row r="47" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B47" s="22"/>
+      <c r="C47" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="D47" s="9"/>
+      <c r="E47" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="F47" s="9"/>
       <c r="G47" s="9"/>
-      <c r="H47" s="17"/>
-    </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B48" s="14"/>
-      <c r="C48" s="9"/>
+      <c r="H47" s="13"/>
+    </row>
+    <row r="48" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="22"/>
+      <c r="C48" s="24" t="s">
+        <v>78</v>
+      </c>
       <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
+      <c r="E48" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="F48" s="9"/>
       <c r="G48" s="9"/>
-      <c r="H48" s="17"/>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B49" s="14"/>
-      <c r="C49" s="16"/>
+      <c r="H48" s="13"/>
+    </row>
+    <row r="49" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="22"/>
+      <c r="C49" s="12" t="s">
+        <v>64</v>
+      </c>
       <c r="D49" s="9"/>
-      <c r="E49" s="9"/>
+      <c r="E49" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="F49" s="9"/>
       <c r="G49" s="9"/>
-      <c r="H49" s="17"/>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B50" s="14"/>
-      <c r="C50" s="16"/>
+      <c r="H49" s="13"/>
+    </row>
+    <row r="50" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B50" s="22"/>
+      <c r="C50" s="12" t="s">
+        <v>65</v>
+      </c>
       <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
+      <c r="E50" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="F50" s="9"/>
       <c r="G50" s="9"/>
-      <c r="H50" s="17"/>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B51" s="15"/>
-      <c r="C51" s="16"/>
+      <c r="H50" s="13"/>
+    </row>
+    <row r="51" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B51" s="22"/>
+      <c r="C51" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="D51" s="9"/>
-      <c r="E51" s="9"/>
+      <c r="E51" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="F51" s="9"/>
       <c r="G51" s="9"/>
-      <c r="H51" s="17"/>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B52" s="9"/>
-      <c r="C52" s="16"/>
+      <c r="H51" s="13"/>
+    </row>
+    <row r="52" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B52" s="22"/>
+      <c r="C52" s="12" t="s">
+        <v>68</v>
+      </c>
       <c r="D52" s="9"/>
-      <c r="E52" s="9"/>
+      <c r="E52" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="F52" s="9"/>
       <c r="G52" s="9"/>
-      <c r="H52" s="17"/>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B53" s="9"/>
-      <c r="C53" s="16"/>
+      <c r="H52" s="13"/>
+    </row>
+    <row r="53" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B53" s="22"/>
+      <c r="C53" s="24" t="s">
+        <v>66</v>
+      </c>
       <c r="D53" s="9"/>
-      <c r="E53" s="9"/>
+      <c r="E53" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="F53" s="9"/>
       <c r="G53" s="9"/>
-      <c r="H53" s="17"/>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B54" s="9"/>
-      <c r="C54" s="16"/>
+      <c r="H53" s="13"/>
+    </row>
+    <row r="54" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B54" s="22"/>
+      <c r="C54" s="24" t="s">
+        <v>83</v>
+      </c>
       <c r="D54" s="9"/>
-      <c r="E54" s="9"/>
+      <c r="E54" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="F54" s="9"/>
       <c r="G54" s="9"/>
-      <c r="H54" s="17"/>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B55" s="9"/>
-      <c r="C55" s="9"/>
+      <c r="H54" s="13"/>
+    </row>
+    <row r="55" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B55" s="22"/>
+      <c r="C55" s="24" t="s">
+        <v>69</v>
+      </c>
       <c r="D55" s="9"/>
-      <c r="E55" s="9"/>
+      <c r="E55" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="F55" s="9"/>
       <c r="G55" s="9"/>
-      <c r="H55" s="17"/>
-    </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B56" s="9"/>
-      <c r="C56" s="9"/>
+      <c r="H55" s="13"/>
+    </row>
+    <row r="56" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B56" s="22"/>
+      <c r="C56" s="24" t="s">
+        <v>84</v>
+      </c>
       <c r="D56" s="9"/>
-      <c r="E56" s="9"/>
-      <c r="F56" s="9"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="G56" s="9"/>
-      <c r="H56" s="17"/>
-    </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B57" s="9"/>
-      <c r="C57" s="9"/>
+      <c r="H56" s="13"/>
+    </row>
+    <row r="57" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B57" s="22"/>
+      <c r="C57" s="24" t="s">
+        <v>70</v>
+      </c>
       <c r="D57" s="9"/>
       <c r="E57" s="9"/>
-      <c r="F57" s="9"/>
+      <c r="F57" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="G57" s="9"/>
-      <c r="H57" s="17"/>
+      <c r="H57" s="13"/>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B58" s="9"/>
-      <c r="C58" s="9"/>
+      <c r="B58" s="22"/>
+      <c r="C58" s="24" t="s">
+        <v>71</v>
+      </c>
       <c r="D58" s="9"/>
       <c r="E58" s="9"/>
-      <c r="F58" s="9"/>
+      <c r="F58" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="G58" s="9"/>
-      <c r="H58" s="17"/>
+      <c r="H58" s="13"/>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B59" s="9"/>
-      <c r="C59" s="9"/>
+      <c r="B59" s="22"/>
+      <c r="C59" s="24" t="s">
+        <v>72</v>
+      </c>
       <c r="D59" s="9"/>
       <c r="E59" s="9"/>
-      <c r="F59" s="9"/>
+      <c r="F59" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="G59" s="9"/>
-      <c r="H59" s="17"/>
+      <c r="H59" s="13"/>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B60" s="9"/>
-      <c r="C60" s="9"/>
+      <c r="B60" s="22"/>
+      <c r="C60" s="24" t="s">
+        <v>73</v>
+      </c>
       <c r="D60" s="9"/>
       <c r="E60" s="9"/>
-      <c r="F60" s="9"/>
+      <c r="F60" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="G60" s="9"/>
-      <c r="H60" s="17"/>
+      <c r="H60" s="13"/>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B61" s="9"/>
-      <c r="C61" s="9"/>
-      <c r="D61" s="9"/>
+      <c r="B61" s="22"/>
+      <c r="C61" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="D61" s="8"/>
       <c r="E61" s="9"/>
-      <c r="F61" s="9"/>
+      <c r="F61" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="G61" s="9"/>
-      <c r="H61" s="17"/>
+      <c r="H61" s="13"/>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B62" s="9"/>
-      <c r="C62" s="9"/>
-      <c r="D62" s="9"/>
+      <c r="B62" s="22"/>
+      <c r="C62" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="D62" s="8"/>
       <c r="E62" s="9"/>
-      <c r="F62" s="9"/>
+      <c r="F62" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="G62" s="9"/>
-      <c r="H62" s="17"/>
+      <c r="H62" s="13"/>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B63" s="9"/>
-      <c r="C63" s="9"/>
-      <c r="D63" s="9"/>
+      <c r="B63" s="22"/>
+      <c r="C63" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="D63" s="8"/>
       <c r="E63" s="9"/>
-      <c r="F63" s="9"/>
+      <c r="F63" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="G63" s="9"/>
-      <c r="H63" s="17"/>
+      <c r="H63" s="13"/>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B64" s="9"/>
-      <c r="C64" s="9"/>
+      <c r="B64" s="22"/>
+      <c r="C64" s="24" t="s">
+        <v>82</v>
+      </c>
       <c r="D64" s="9"/>
       <c r="E64" s="9"/>
-      <c r="F64" s="9"/>
+      <c r="F64" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="G64" s="9"/>
-      <c r="H64" s="17"/>
+      <c r="H64" s="13"/>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B65" s="9"/>
-      <c r="C65" s="9"/>
+      <c r="B65" s="22"/>
+      <c r="C65" s="24" t="s">
+        <v>80</v>
+      </c>
       <c r="D65" s="9"/>
       <c r="E65" s="9"/>
-      <c r="F65" s="9"/>
+      <c r="F65" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="G65" s="9"/>
-      <c r="H65" s="17"/>
+      <c r="H65" s="13"/>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B66" s="9"/>
-      <c r="C66" s="9"/>
+      <c r="B66" s="22"/>
+      <c r="C66" s="24" t="s">
+        <v>81</v>
+      </c>
       <c r="D66" s="9"/>
       <c r="E66" s="9"/>
-      <c r="F66" s="9"/>
+      <c r="F66" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="G66" s="9"/>
-      <c r="H66" s="17"/>
+      <c r="H66" s="13"/>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B67" s="9"/>
-      <c r="C67" s="9"/>
-      <c r="D67" s="9"/>
+      <c r="B67" s="22"/>
+      <c r="C67" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D67" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="E67" s="9"/>
       <c r="F67" s="9"/>
       <c r="G67" s="9"/>
-      <c r="H67" s="17"/>
+      <c r="H67" s="13"/>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B68" s="9"/>
-      <c r="C68" s="9"/>
-      <c r="D68" s="9"/>
+      <c r="B68" s="22"/>
+      <c r="C68" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D68" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="E68" s="9"/>
       <c r="F68" s="9"/>
       <c r="G68" s="9"/>
-      <c r="H68" s="9"/>
+      <c r="H68" s="13"/>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B69" s="9"/>
-      <c r="C69" s="9"/>
-      <c r="D69" s="9"/>
+      <c r="B69" s="23"/>
+      <c r="C69" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D69" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="E69" s="9"/>
       <c r="F69" s="9"/>
       <c r="G69" s="9"/>
-      <c r="H69" s="9"/>
+      <c r="H69" s="13"/>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B70" s="9"/>
@@ -1487,7 +1809,7 @@
       <c r="E70" s="9"/>
       <c r="F70" s="9"/>
       <c r="G70" s="9"/>
-      <c r="H70" s="9"/>
+      <c r="H70" s="13"/>
     </row>
     <row r="71" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B71" s="9"/>
@@ -1496,7 +1818,7 @@
       <c r="E71" s="9"/>
       <c r="F71" s="9"/>
       <c r="G71" s="9"/>
-      <c r="H71" s="9"/>
+      <c r="H71" s="13"/>
     </row>
     <row r="72" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B72" s="9"/>
@@ -1505,7 +1827,7 @@
       <c r="E72" s="9"/>
       <c r="F72" s="9"/>
       <c r="G72" s="9"/>
-      <c r="H72" s="9"/>
+      <c r="H72" s="13"/>
     </row>
     <row r="73" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B73" s="9"/>
@@ -1561,76 +1883,165 @@
       <c r="G78" s="9"/>
       <c r="H78" s="9"/>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A83" s="19" t="s">
+    <row r="79" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B79" s="9"/>
+      <c r="C79" s="9"/>
+      <c r="D79" s="9"/>
+      <c r="E79" s="9"/>
+      <c r="F79" s="9"/>
+      <c r="G79" s="9"/>
+      <c r="H79" s="9"/>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B80" s="9"/>
+      <c r="C80" s="9"/>
+      <c r="D80" s="9"/>
+      <c r="E80" s="9"/>
+      <c r="F80" s="9"/>
+      <c r="G80" s="9"/>
+      <c r="H80" s="9"/>
+    </row>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B81" s="9"/>
+      <c r="C81" s="9"/>
+      <c r="D81" s="9"/>
+      <c r="E81" s="9"/>
+      <c r="F81" s="9"/>
+      <c r="G81" s="9"/>
+      <c r="H81" s="9"/>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B82" s="9"/>
+      <c r="C82" s="9"/>
+      <c r="D82" s="9"/>
+      <c r="E82" s="9"/>
+      <c r="F82" s="9"/>
+      <c r="G82" s="9"/>
+      <c r="H82" s="9"/>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B83" s="9"/>
+      <c r="C83" s="9"/>
+      <c r="D83" s="9"/>
+      <c r="E83" s="9"/>
+      <c r="F83" s="9"/>
+      <c r="G83" s="9"/>
+      <c r="H83" s="9"/>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B84" s="9"/>
+      <c r="C84" s="9"/>
+      <c r="D84" s="9"/>
+      <c r="E84" s="9"/>
+      <c r="F84" s="9"/>
+      <c r="G84" s="9"/>
+      <c r="H84" s="9"/>
+    </row>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B85" s="9"/>
+      <c r="C85" s="9"/>
+      <c r="D85" s="9"/>
+      <c r="E85" s="9"/>
+      <c r="F85" s="9"/>
+      <c r="G85" s="9"/>
+      <c r="H85" s="9"/>
+    </row>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B86" s="9"/>
+      <c r="C86" s="9"/>
+      <c r="D86" s="9"/>
+      <c r="E86" s="9"/>
+      <c r="F86" s="9"/>
+      <c r="G86" s="9"/>
+      <c r="H86" s="9"/>
+    </row>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B87" s="9"/>
+      <c r="C87" s="9"/>
+      <c r="D87" s="9"/>
+      <c r="E87" s="9"/>
+      <c r="F87" s="9"/>
+      <c r="G87" s="9"/>
+      <c r="H87" s="9"/>
+    </row>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B88" s="9"/>
+      <c r="C88" s="9"/>
+      <c r="D88" s="9"/>
+      <c r="E88" s="9"/>
+      <c r="F88" s="9"/>
+      <c r="G88" s="9"/>
+      <c r="H88" s="9"/>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B83" s="20"/>
-      <c r="C83" s="21"/>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A84" s="22" t="s">
+      <c r="B98" s="16"/>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B84" s="22" t="s">
+      <c r="B99" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="C84" s="23" t="s">
+      <c r="C99" s="18" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="48" x14ac:dyDescent="0.2">
-      <c r="A85" s="22">
+    <row r="100" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A100" s="17">
         <v>1</v>
       </c>
-      <c r="B85" s="24" t="s">
+      <c r="B100" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C85" s="23">
+      <c r="C100" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A86" s="23">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" s="18">
         <v>2</v>
       </c>
-      <c r="B86" s="24" t="s">
+      <c r="B101" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="C86" s="23">
+      <c r="C101" s="18">
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A87" s="23">
+    <row r="102" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A102" s="18">
         <v>3</v>
       </c>
-      <c r="B87" s="24" t="s">
+      <c r="B102" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C87" s="23">
+      <c r="C102" s="18">
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A88" s="23">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103" s="18">
         <v>4</v>
       </c>
-      <c r="B88" s="24" t="s">
+      <c r="B103" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="C88" s="23">
+      <c r="C103" s="18">
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A89" s="23">
+    <row r="104" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A104" s="18">
         <v>5</v>
       </c>
-      <c r="B89" s="24" t="s">
+      <c r="B104" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C89" s="23">
+      <c r="C104" s="18">
         <v>5</v>
       </c>
     </row>
@@ -1638,7 +2049,7 @@
   <mergeCells count="3">
     <mergeCell ref="B2:B9"/>
     <mergeCell ref="B10:B23"/>
-    <mergeCell ref="B24:B51"/>
+    <mergeCell ref="B24:B69"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>